<commit_message>
My changes to Python and some small bugfixes in the database
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigBP.xlsx
+++ b/ConfigFiles/ConfigBP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DARKO\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speet\DARKO\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07520A6B-C203-4CB4-80D6-E05B8185FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD97CA5-6498-4C46-B76E-05777244E45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="169">
   <si>
     <t>Default value</t>
   </si>
@@ -539,9 +539,6 @@
   </si>
   <si>
     <t>BP/Interconnections/NTC/NTC.csv</t>
-  </si>
-  <si>
-    <t>BP/Interconnections/CBF/CBF.csv</t>
   </si>
 </sst>
 </file>
@@ -732,7 +729,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -748,7 +745,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1071,24 +1068,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>118</v>
       </c>
@@ -1100,7 +1097,7 @@
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1110,8 +1107,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="31" t="s">
         <v>119</v>
       </c>
@@ -1122,7 +1119,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1132,7 +1129,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1146,7 +1143,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1155,20 +1152,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1180,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -1197,7 +1194,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1211,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1225,7 +1222,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>100</v>
       </c>
@@ -1248,17 +1245,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1266,13 +1263,13 @@
         <v>36</v>
       </c>
       <c r="C31" s="18">
-        <v>42370</v>
+        <v>43831</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1280,13 +1277,13 @@
         <v>36</v>
       </c>
       <c r="C32" s="18">
-        <v>42373</v>
+        <v>44196</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -1311,24 +1308,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1356,26 +1353,26 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>133</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>134</v>
       </c>
@@ -1409,7 +1406,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>135</v>
       </c>
@@ -1424,7 +1421,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>136</v>
       </c>
@@ -1442,7 +1439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>127</v>
       </c>
@@ -1459,7 +1456,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>128</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>122</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>130</v>
       </c>
@@ -1512,7 +1509,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>131</v>
       </c>
@@ -1524,7 +1521,7 @@
       </c>
       <c r="D70" s="19"/>
     </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>132</v>
       </c>
@@ -1538,21 +1535,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="20" t="s">
-        <v>169</v>
-      </c>
+      <c r="C72" s="20"/>
       <c r="D72" s="19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
@@ -1563,7 +1558,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>149</v>
       </c>
@@ -1571,10 +1566,10 @@
         <v>0</v>
       </c>
       <c r="F74" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>150</v>
       </c>
@@ -1585,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>147</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>148</v>
       </c>
@@ -1607,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>145</v>
       </c>
@@ -1618,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>146</v>
       </c>
@@ -1629,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>143</v>
       </c>
@@ -1640,7 +1635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>144</v>
       </c>
@@ -1651,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>159</v>
       </c>
@@ -1660,7 +1655,7 @@
       </c>
       <c r="C82" s="20"/>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>160</v>
       </c>
@@ -1669,13 +1664,13 @@
       </c>
       <c r="C83" s="20"/>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="22" t="s">
         <v>125</v>
       </c>
@@ -1692,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>45</v>
       </c>
@@ -1709,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="31"/>
       <c r="B89" s="6" t="s">
         <v>20</v>
@@ -1724,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="31"/>
       <c r="B90" s="6" t="s">
         <v>106</v>
@@ -1739,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="31"/>
       <c r="B91" s="6" t="s">
         <v>101</v>
@@ -1754,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="31"/>
       <c r="B92" s="6" t="s">
         <v>3</v>
@@ -1769,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="31"/>
       <c r="B93" s="6" t="s">
         <v>114</v>
@@ -1784,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="31"/>
       <c r="B94" s="6" t="s">
         <v>29</v>
@@ -1799,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="31"/>
       <c r="B95" s="6" t="s">
         <v>14</v>
@@ -1814,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="31"/>
       <c r="B96" s="6" t="s">
         <v>4</v>
@@ -1829,13 +1824,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="31"/>
       <c r="B97" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>21</v>
@@ -1844,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="31"/>
       <c r="B98" s="6" t="s">
         <v>5</v>
@@ -1859,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="31"/>
       <c r="B99" s="6" t="s">
         <v>7</v>
@@ -1874,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="31"/>
       <c r="B100" s="6" t="s">
         <v>9</v>
@@ -1889,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="31"/>
       <c r="B101" s="6" t="s">
         <v>10</v>
@@ -1904,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="31"/>
       <c r="B102" s="6" t="s">
         <v>26</v>
@@ -1919,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="6" t="s">
         <v>11</v>
       </c>
@@ -1933,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="6" t="s">
         <v>12</v>
       </c>
@@ -1947,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="6" t="s">
         <v>18</v>
       </c>
@@ -1961,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="6" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="6" t="s">
         <v>111</v>
       </c>
@@ -1989,13 +1984,13 @@
         <v>28</v>
       </c>
       <c r="F107" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="6" t="s">
         <v>13</v>
       </c>
@@ -2009,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="6" t="s">
         <v>129</v>
       </c>
@@ -2023,17 +2018,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="9"/>
       <c r="C110" s="15"/>
     </row>
-    <row r="111" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>1</v>
       </c>
@@ -2044,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>59</v>
       </c>
@@ -2058,7 +2053,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>60</v>
       </c>
@@ -2072,7 +2067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>62</v>
       </c>
@@ -2083,30 +2078,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:3" s="10" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:3" s="10" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="9"/>
       <c r="C129" s="15"/>
     </row>
-    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="24" t="s">
         <v>70</v>
       </c>
@@ -2114,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="24" t="s">
         <v>71</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="24" t="s">
         <v>72</v>
       </c>
@@ -2130,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="24" t="s">
         <v>73</v>
       </c>
@@ -2138,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="24" t="s">
         <v>74</v>
       </c>
@@ -2146,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B138" s="24" t="s">
         <v>75</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="24" t="s">
         <v>76</v>
       </c>
@@ -2162,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="24" t="s">
         <v>77</v>
       </c>
@@ -2170,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="24" t="s">
         <v>78</v>
       </c>
@@ -2178,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="24" t="s">
         <v>79</v>
       </c>
@@ -2186,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="24" t="s">
         <v>80</v>
       </c>
@@ -2194,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="24" t="s">
         <v>81</v>
       </c>
@@ -2202,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="24" t="s">
         <v>82</v>
       </c>
@@ -2210,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="29" t="s">
         <v>83</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="24" t="s">
         <v>84</v>
       </c>
@@ -2226,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="29" t="s">
         <v>153</v>
       </c>
@@ -2234,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="29" t="s">
         <v>154</v>
       </c>
@@ -2242,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B150" s="29" t="s">
         <v>155</v>
       </c>
@@ -2250,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B151" s="29" t="s">
         <v>156</v>
       </c>
@@ -2258,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B152" s="29" t="s">
         <v>157</v>
       </c>
@@ -2266,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B153" s="29" t="s">
         <v>158</v>
       </c>
@@ -2274,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F166" s="2"/>
     </row>
   </sheetData>
@@ -2376,14 +2371,14 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -2394,7 +2389,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2405,7 +2400,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2425,12 +2420,12 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26"/>
       <c r="B1" s="26" t="s">
         <v>85</v>
@@ -2475,7 +2470,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>70</v>
       </c>
@@ -2522,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
@@ -2569,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>72</v>
       </c>
@@ -2616,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
@@ -2663,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
@@ -2710,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>75</v>
       </c>
@@ -2757,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>76</v>
       </c>
@@ -2804,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>77</v>
       </c>
@@ -2851,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>78</v>
       </c>
@@ -2898,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -2945,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
@@ -2992,7 +2987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>81</v>
       </c>
@@ -3039,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>82</v>
       </c>
@@ -3086,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>83</v>
       </c>
@@ -3133,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>84</v>
       </c>

</xml_diff>